<commit_message>
Added VLC survey results
</commit_message>
<xml_diff>
--- a/03_Outputs/Course_Evaluation/Overall_Evaluation_2022.xlsx
+++ b/03_Outputs/Course_Evaluation/Overall_Evaluation_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\htdocs\Project_SPARTA_PH\03_Outputs\Course_Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7C7502-6171-4708-91B2-6F6A8A4C549E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43509867-1F0D-474A-9278-308EDF6EFF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19200" windowHeight="11760" tabRatio="767" activeTab="3" xr2:uid="{71074A19-0A8E-4A39-A280-0FF2D7A6D92C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19200" windowHeight="11760" tabRatio="767" activeTab="2" xr2:uid="{71074A19-0A8E-4A39-A280-0FF2D7A6D92C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Rating" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Heatmap!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Overall Rating'!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Overall Rating'!$E$37:$E$64</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Overall Rating'!$F$37:$F$64</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Overall Rating'!$E$37:$E$64</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Overall Rating'!$F$37:$F$64</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Overall Rating'!$F$2:$F$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId6"/>
+    <pivotCache cacheId="45" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,8 +46,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{DA6F7714-E7E9-4A7C-A854-4A4CF3D759C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+244</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="96">
   <si>
     <t>Course Description</t>
   </si>
@@ -304,9 +338,6 @@
     <t>Statistical Techniques</t>
   </si>
   <si>
-    <t>As of November 2022</t>
-  </si>
-  <si>
     <t>Max_NPS</t>
   </si>
   <si>
@@ -324,6 +355,21 @@
   <si>
     <t>Rank</t>
   </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Methods &amp; Logistics</t>
+  </si>
+  <si>
+    <t>Overall Ave</t>
+  </si>
+  <si>
+    <t>Respondents_VLC</t>
+  </si>
 </sst>
 </file>
 
@@ -333,7 +379,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mmm\ yy"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,18 +490,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -672,7 +730,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -782,7 +840,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -833,9 +890,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -843,78 +945,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="29">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1045,6 +1075,78 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1313,7 +1415,7 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{0AF79F22-9AD9-4B59-AF48-719D17F8F139}">
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{0AF79F22-9AD9-4B59-AF48-719D17F8F139}" formatIdx="0">
           <cx:spPr>
             <a:gradFill flip="none" rotWithShape="1">
               <a:gsLst>
@@ -1350,14 +1452,6 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1" hidden="1">
-        <cx:valScaling max="1" min="0.20000000000000001"/>
-        <cx:tickLabels/>
-      </cx:axis>
     </cx:plotArea>
   </cx:chart>
 </cx:chartSpace>
@@ -1368,7 +1462,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1456,7 +1550,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1546,7 +1640,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5610,7 +5704,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E6C9730-EF2D-4F21-9966-607D837C00DD}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Competency">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E6C9730-EF2D-4F21-9966-607D837C00DD}" name="PivotTable4" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Competency">
   <location ref="A3:F19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField numFmtId="165" showAll="0"/>
@@ -5785,10 +5879,10 @@
     <dataField name="Average Course_Rating" fld="5" subtotal="average" baseField="1" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="14">
-    <format dxfId="13">
+    <format dxfId="28">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -5801,10 +5895,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="26">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -5817,10 +5911,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="24">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -5833,26 +5927,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="22">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="20">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -5865,10 +5959,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -5883,23 +5977,23 @@
     </format>
   </formats>
   <conditionalFormats count="2">
+    <conditionalFormat priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat priority="3">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
               <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="5">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="1"/>
             </reference>
           </references>
         </pivotArea>
@@ -12135,77 +12229,77 @@
     <sortCondition ref="D2:D27"/>
   </sortState>
   <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="14" priority="32" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="31" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="12" priority="30" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="29" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="10" priority="28" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="8" priority="26" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="25" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="(blank)">
+    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="(blank)">
       <formula>NOT(ISERROR(SEARCH("(blank)",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
       <formula>"(blank)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B1048576 B1:B35 B65">
-    <cfRule type="duplicateValues" dxfId="14" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F31">
     <cfRule type="colorScale" priority="43">
@@ -12308,27 +12402,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B480025-07C2-4AD3-A6F8-AFC279FCF808}">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B480025-07C2-4AD3-A6F8-AFC279FCF808}">
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.75" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="48.625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.25" style="29" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="29"/>
+    <col min="5" max="5" width="48.625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.25" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="18.5" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="12" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.375" style="77" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.5" style="68" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="68" customWidth="1"/>
+    <col min="13" max="13" width="16.25" style="68" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="68" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.375" style="29" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="30" t="s">
         <v>66</v>
       </c>
@@ -12350,9 +12451,24 @@
       <c r="H1" s="36" t="s">
         <v>63</v>
       </c>
+      <c r="J1" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="63" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
+    <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
         <v>1</v>
       </c>
       <c r="B2" s="37">
@@ -12379,9 +12495,24 @@
         <f>VLOOKUP(D2,'Overall Rating'!C:G,5,FALSE)</f>
         <v>11861</v>
       </c>
+      <c r="J2" s="66">
+        <v>49</v>
+      </c>
+      <c r="K2" s="64">
+        <v>4.8816326530612244</v>
+      </c>
+      <c r="L2" s="64">
+        <v>4.9142857142857137</v>
+      </c>
+      <c r="M2" s="64">
+        <v>4.8326530612244891</v>
+      </c>
+      <c r="N2" s="64">
+        <v>4.8761904761904757</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
+    <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
         <v>2</v>
       </c>
       <c r="B3" s="37">
@@ -12408,9 +12539,24 @@
         <f>VLOOKUP(D3,'Overall Rating'!C:G,5,FALSE)</f>
         <v>64</v>
       </c>
+      <c r="J3" s="66">
+        <v>108</v>
+      </c>
+      <c r="K3" s="64">
+        <v>4.590740740740741</v>
+      </c>
+      <c r="L3" s="64">
+        <v>4.6685185185185185</v>
+      </c>
+      <c r="M3" s="64">
+        <v>4.6296296296296298</v>
+      </c>
+      <c r="N3" s="64">
+        <v>4.6296296296296298</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
+    <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
         <v>3</v>
       </c>
       <c r="B4" s="37">
@@ -12437,9 +12583,24 @@
         <f>VLOOKUP(D4,'Overall Rating'!C:G,5,FALSE)</f>
         <v>3497</v>
       </c>
+      <c r="J4" s="66">
+        <v>325</v>
+      </c>
+      <c r="K4" s="64">
+        <v>4.5021538461538455</v>
+      </c>
+      <c r="L4" s="64">
+        <v>4.6646153846153844</v>
+      </c>
+      <c r="M4" s="64">
+        <v>4.5889230769230762</v>
+      </c>
+      <c r="N4" s="64">
+        <v>4.585230769230769</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
         <v>4</v>
       </c>
       <c r="B5" s="37">
@@ -12466,9 +12627,24 @@
         <f>VLOOKUP(D5,'Overall Rating'!C:G,5,FALSE)</f>
         <v>553</v>
       </c>
+      <c r="J5" s="66">
+        <v>190</v>
+      </c>
+      <c r="K5" s="64">
+        <v>4.5657744360902255</v>
+      </c>
+      <c r="L5" s="64">
+        <v>4.7681654135338345</v>
+      </c>
+      <c r="M5" s="64">
+        <v>4.7224661654135343</v>
+      </c>
+      <c r="N5" s="64">
+        <v>4.6854686716791978</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
+    <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
         <v>5</v>
       </c>
       <c r="B6" s="37">
@@ -12495,9 +12671,24 @@
         <f>VLOOKUP(D6,'Overall Rating'!C:G,5,FALSE)</f>
         <v>718</v>
       </c>
+      <c r="J6" s="66">
+        <v>247</v>
+      </c>
+      <c r="K6" s="64">
+        <v>4.5635627530364369</v>
+      </c>
+      <c r="L6" s="64">
+        <v>4.6696356275303641</v>
+      </c>
+      <c r="M6" s="64">
+        <v>4.6449392712550619</v>
+      </c>
+      <c r="N6" s="64">
+        <v>4.6260458839406216</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
+    <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
         <v>6</v>
       </c>
       <c r="B7" s="37">
@@ -12524,9 +12715,29 @@
         <f>VLOOKUP(D7,'Overall Rating'!C:G,5,FALSE)</f>
         <v>2412</v>
       </c>
+      <c r="J7" s="66">
+        <v>280</v>
+      </c>
+      <c r="K7" s="64">
+        <v>4.3335714285714282</v>
+      </c>
+      <c r="L7" s="64">
+        <v>4.4707142857142861</v>
+      </c>
+      <c r="M7" s="64">
+        <v>4.4764285714285723</v>
+      </c>
+      <c r="N7" s="64">
+        <v>4.4269047619047628</v>
+      </c>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
     </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44">
+    <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
         <v>7</v>
       </c>
       <c r="B8" s="37">
@@ -12553,9 +12764,29 @@
         <f>VLOOKUP(D8,'Overall Rating'!C:G,5,FALSE)</f>
         <v>129</v>
       </c>
+      <c r="J8" s="66">
+        <v>250</v>
+      </c>
+      <c r="K8" s="64">
+        <v>4.4605577689243026</v>
+      </c>
+      <c r="L8" s="64">
+        <v>4.5617529880478092</v>
+      </c>
+      <c r="M8" s="64">
+        <v>4.5752988047808767</v>
+      </c>
+      <c r="N8" s="64">
+        <v>4.5325365205843289</v>
+      </c>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
         <v>8</v>
       </c>
       <c r="B9" s="37">
@@ -12582,9 +12813,29 @@
         <f>VLOOKUP(D9,'Overall Rating'!C:G,5,FALSE)</f>
         <v>1054</v>
       </c>
+      <c r="J9" s="66">
+        <v>274</v>
+      </c>
+      <c r="K9" s="64">
+        <v>4.4631270999884141</v>
+      </c>
+      <c r="L9" s="64">
+        <v>4.6114760746147603</v>
+      </c>
+      <c r="M9" s="64">
+        <v>4.6511209593326379</v>
+      </c>
+      <c r="N9" s="64">
+        <v>4.5752413779786032</v>
+      </c>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
     </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
+    <row r="10" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
         <v>9</v>
       </c>
       <c r="B10" s="37">
@@ -12611,9 +12862,29 @@
         <f>VLOOKUP(D10,'Overall Rating'!C:G,5,FALSE)</f>
         <v>881</v>
       </c>
+      <c r="J10" s="66">
+        <v>281</v>
+      </c>
+      <c r="K10" s="64">
+        <v>4.7010676156583626</v>
+      </c>
+      <c r="L10" s="64">
+        <v>4.7850533807829176</v>
+      </c>
+      <c r="M10" s="64">
+        <v>4.7131672597864762</v>
+      </c>
+      <c r="N10" s="64">
+        <v>4.7330960854092519</v>
+      </c>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
     </row>
-    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
+    <row r="11" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43">
         <v>10</v>
       </c>
       <c r="B11" s="37">
@@ -12640,9 +12911,29 @@
         <f>VLOOKUP(D11,'Overall Rating'!C:G,5,FALSE)</f>
         <v>156</v>
       </c>
+      <c r="J11" s="66">
+        <v>150</v>
+      </c>
+      <c r="K11" s="64">
+        <v>4.6371394284190419</v>
+      </c>
+      <c r="L11" s="64">
+        <v>4.7379394639761765</v>
+      </c>
+      <c r="M11" s="64">
+        <v>4.6720476465620697</v>
+      </c>
+      <c r="N11" s="64">
+        <v>4.6823755129857627</v>
+      </c>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
+    <row r="12" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
         <v>11</v>
       </c>
       <c r="B12" s="37">
@@ -12669,9 +12960,29 @@
         <f>VLOOKUP(D12,'Overall Rating'!C:G,5,FALSE)</f>
         <v>284</v>
       </c>
+      <c r="J12" s="66">
+        <v>313</v>
+      </c>
+      <c r="K12" s="64">
+        <v>4.7194888178913743</v>
+      </c>
+      <c r="L12" s="64">
+        <v>4.788498402555911</v>
+      </c>
+      <c r="M12" s="64">
+        <v>4.7015974440894563</v>
+      </c>
+      <c r="N12" s="64">
+        <v>4.7365282215122475</v>
+      </c>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
     </row>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
+    <row r="13" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43">
         <v>12</v>
       </c>
       <c r="B13" s="37">
@@ -12698,9 +13009,24 @@
         <f>VLOOKUP(D13,'Overall Rating'!C:G,5,FALSE)</f>
         <v>246</v>
       </c>
+      <c r="J13" s="66">
+        <v>193</v>
+      </c>
+      <c r="K13" s="64">
+        <v>4.5654450261780095</v>
+      </c>
+      <c r="L13" s="64">
+        <v>4.6471204188481678</v>
+      </c>
+      <c r="M13" s="64">
+        <v>4.6272251308900518</v>
+      </c>
+      <c r="N13" s="64">
+        <v>4.6132635253054097</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
+    <row r="14" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
         <v>13</v>
       </c>
       <c r="B14" s="37">
@@ -12727,9 +13053,14 @@
         <f>VLOOKUP(D14,'Overall Rating'!C:G,5,FALSE)</f>
         <v>119</v>
       </c>
+      <c r="J14" s="66"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
     </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
+    <row r="15" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
         <v>14</v>
       </c>
       <c r="B15" s="37">
@@ -12756,9 +13087,24 @@
         <f>VLOOKUP(D15,'Overall Rating'!C:G,5,FALSE)</f>
         <v>76</v>
       </c>
+      <c r="J15" s="66">
+        <v>165</v>
+      </c>
+      <c r="K15" s="64">
+        <v>4.4475324675324668</v>
+      </c>
+      <c r="L15" s="64">
+        <v>4.5246753246753242</v>
+      </c>
+      <c r="M15" s="64">
+        <v>4.5697402597402599</v>
+      </c>
+      <c r="N15" s="64">
+        <v>4.5139826839826842</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
+    <row r="16" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
         <v>15</v>
       </c>
       <c r="B16" s="37">
@@ -12785,9 +13131,24 @@
         <f>VLOOKUP(D16,'Overall Rating'!C:G,5,FALSE)</f>
         <v>34</v>
       </c>
+      <c r="J16" s="66">
+        <v>165</v>
+      </c>
+      <c r="K16" s="64">
+        <v>4.7157575757575758</v>
+      </c>
+      <c r="L16" s="64">
+        <v>4.7727272727272734</v>
+      </c>
+      <c r="M16" s="64">
+        <v>4.7230303030303036</v>
+      </c>
+      <c r="N16" s="64">
+        <v>4.7371717171717176</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
+    <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43">
         <v>16</v>
       </c>
       <c r="B17" s="37">
@@ -12814,9 +13175,24 @@
         <f>VLOOKUP(D17,'Overall Rating'!C:G,5,FALSE)</f>
         <v>2</v>
       </c>
+      <c r="J17" s="66">
+        <v>70</v>
+      </c>
+      <c r="K17" s="64">
+        <v>4.6552380952380954</v>
+      </c>
+      <c r="L17" s="64">
+        <v>4.7732467532467533</v>
+      </c>
+      <c r="M17" s="64">
+        <v>4.7056277056277054</v>
+      </c>
+      <c r="N17" s="64">
+        <v>4.7113708513708517</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+    <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
         <v>17</v>
       </c>
       <c r="B18" s="37">
@@ -12843,9 +13219,24 @@
         <f>VLOOKUP(D18,'Overall Rating'!C:G,5,FALSE)</f>
         <v>20</v>
       </c>
+      <c r="J18" s="66">
+        <v>293</v>
+      </c>
+      <c r="K18" s="64">
+        <v>4.5257678986228642</v>
+      </c>
+      <c r="L18" s="64">
+        <v>4.6583554560035401</v>
+      </c>
+      <c r="M18" s="64">
+        <v>4.6551694458271111</v>
+      </c>
+      <c r="N18" s="64">
+        <v>4.6130976001511712</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
+    <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
         <v>18</v>
       </c>
       <c r="B19" s="37">
@@ -12872,9 +13263,24 @@
         <f>VLOOKUP(D19,'Overall Rating'!C:G,5,FALSE)</f>
         <v>229</v>
       </c>
+      <c r="J19" s="66">
+        <v>148</v>
+      </c>
+      <c r="K19" s="64">
+        <v>4.6292721855713976</v>
+      </c>
+      <c r="L19" s="64">
+        <v>4.7607203660353274</v>
+      </c>
+      <c r="M19" s="64">
+        <v>4.7151308789104061</v>
+      </c>
+      <c r="N19" s="64">
+        <v>4.701707810172377</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
+    <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43">
         <v>19</v>
       </c>
       <c r="B20" s="37">
@@ -12901,9 +13307,24 @@
         <f>VLOOKUP(D20,'Overall Rating'!C:G,5,FALSE)</f>
         <v>72</v>
       </c>
+      <c r="J20" s="66">
+        <v>207</v>
+      </c>
+      <c r="K20" s="64">
+        <v>4.7221772834512965</v>
+      </c>
+      <c r="L20" s="64">
+        <v>4.7902061566116165</v>
+      </c>
+      <c r="M20" s="64">
+        <v>4.7159055162341312</v>
+      </c>
+      <c r="N20" s="64">
+        <v>4.7427629854323481</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44">
+    <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
         <v>20</v>
       </c>
       <c r="B21" s="37">
@@ -12930,9 +13351,24 @@
         <f>VLOOKUP(D21,'Overall Rating'!C:G,5,FALSE)</f>
         <v>14</v>
       </c>
+      <c r="J21" s="66">
+        <v>81</v>
+      </c>
+      <c r="K21" s="64">
+        <v>4.7638024691358023</v>
+      </c>
+      <c r="L21" s="64">
+        <v>4.8364938271604938</v>
+      </c>
+      <c r="M21" s="64">
+        <v>4.7128395061728394</v>
+      </c>
+      <c r="N21" s="64">
+        <v>4.7710452674897121</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44">
+    <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
         <v>21</v>
       </c>
       <c r="B22" s="37">
@@ -12959,9 +13395,24 @@
         <f>VLOOKUP(D22,'Overall Rating'!C:G,5,FALSE)</f>
         <v>300</v>
       </c>
+      <c r="J22" s="66">
+        <v>203</v>
+      </c>
+      <c r="K22" s="64">
+        <v>4.6431372549019603</v>
+      </c>
+      <c r="L22" s="64">
+        <v>4.7519607843137255</v>
+      </c>
+      <c r="M22" s="64">
+        <v>4.6421568627450984</v>
+      </c>
+      <c r="N22" s="64">
+        <v>4.6790849673202617</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44">
+    <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43">
         <v>22</v>
       </c>
       <c r="B23" s="37">
@@ -12988,9 +13439,24 @@
         <f>VLOOKUP(D23,'Overall Rating'!C:G,5,FALSE)</f>
         <v>487</v>
       </c>
+      <c r="J23" s="66">
+        <v>184</v>
+      </c>
+      <c r="K23" s="64">
+        <v>4.6021739130434778</v>
+      </c>
+      <c r="L23" s="64">
+        <v>4.6423913043478269</v>
+      </c>
+      <c r="M23" s="64">
+        <v>4.6347826086956525</v>
+      </c>
+      <c r="N23" s="64">
+        <v>4.6264492753623188</v>
+      </c>
     </row>
-    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44">
+    <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="43">
         <v>23</v>
       </c>
       <c r="B24" s="37">
@@ -13017,9 +13483,24 @@
         <f>VLOOKUP(D24,'Overall Rating'!C:G,5,FALSE)</f>
         <v>416</v>
       </c>
+      <c r="J24" s="66">
+        <v>192</v>
+      </c>
+      <c r="K24" s="64">
+        <v>4.6645833333333337</v>
+      </c>
+      <c r="L24" s="64">
+        <v>4.7333333333333325</v>
+      </c>
+      <c r="M24" s="64">
+        <v>4.7177083333333334</v>
+      </c>
+      <c r="N24" s="64">
+        <v>4.7052083333333341</v>
+      </c>
     </row>
-    <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44">
+    <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43">
         <v>24</v>
       </c>
       <c r="B25" s="37">
@@ -13046,9 +13527,24 @@
         <f>VLOOKUP(D25,'Overall Rating'!C:G,5,FALSE)</f>
         <v>204</v>
       </c>
+      <c r="J25" s="66">
+        <v>176</v>
+      </c>
+      <c r="K25" s="64">
+        <v>4.6734463276836156</v>
+      </c>
+      <c r="L25" s="64">
+        <v>4.7378531073446322</v>
+      </c>
+      <c r="M25" s="64">
+        <v>4.6757062146892654</v>
+      </c>
+      <c r="N25" s="64">
+        <v>4.6956685499058377</v>
+      </c>
     </row>
-    <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44">
+    <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="43">
         <v>25</v>
       </c>
       <c r="B26" s="37">
@@ -13075,9 +13571,24 @@
         <f>VLOOKUP(D26,'Overall Rating'!C:G,5,FALSE)</f>
         <v>221</v>
       </c>
+      <c r="J26" s="66">
+        <v>122</v>
+      </c>
+      <c r="K26" s="64">
+        <v>4.7016393442622952</v>
+      </c>
+      <c r="L26" s="64">
+        <v>4.7524590163934421</v>
+      </c>
+      <c r="M26" s="64">
+        <v>4.695081967213115</v>
+      </c>
+      <c r="N26" s="64">
+        <v>4.7163934426229508</v>
+      </c>
     </row>
-    <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44">
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43">
         <v>26</v>
       </c>
       <c r="B27" s="37">
@@ -13104,9 +13615,24 @@
         <f>VLOOKUP(D27,'Overall Rating'!C:G,5,FALSE)</f>
         <v>302</v>
       </c>
+      <c r="J27" s="66">
+        <v>52</v>
+      </c>
+      <c r="K27" s="64">
+        <v>4.611538461538462</v>
+      </c>
+      <c r="L27" s="64">
+        <v>4.7115384615384617</v>
+      </c>
+      <c r="M27" s="64">
+        <v>4.6423076923076918</v>
+      </c>
+      <c r="N27" s="64">
+        <v>4.6551282051282046</v>
+      </c>
     </row>
-    <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44">
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="43">
         <v>27</v>
       </c>
       <c r="B28" s="37">
@@ -13133,38 +13659,68 @@
         <f>VLOOKUP(D28,'Overall Rating'!C:G,5,FALSE)</f>
         <v>314</v>
       </c>
+      <c r="J28" s="66">
+        <v>97</v>
+      </c>
+      <c r="K28" s="64">
+        <v>4.6144329896907221</v>
+      </c>
+      <c r="L28" s="64">
+        <v>4.6721649484536085</v>
+      </c>
+      <c r="M28" s="64">
+        <v>4.7175257731958764</v>
+      </c>
+      <c r="N28" s="64">
+        <v>4.6680412371134024</v>
+      </c>
     </row>
-    <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44">
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43">
         <v>28</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="69">
         <v>44300</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="72">
         <f>VLOOKUP(D29,'Overall Rating'!C:G,3,FALSE)</f>
         <v>0.93142857142857138</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="73">
         <f>VLOOKUP(D29,'Overall Rating'!C:G,4,FALSE)</f>
         <v>9.3542857142857141</v>
       </c>
-      <c r="H29" s="41">
+      <c r="H29" s="74">
         <f>VLOOKUP(D29,'Overall Rating'!C:G,5,FALSE)</f>
         <v>175</v>
       </c>
+      <c r="J29" s="75">
+        <v>93</v>
+      </c>
+      <c r="K29" s="76">
+        <v>4.655913978494624</v>
+      </c>
+      <c r="L29" s="76">
+        <v>4.7763440860215054</v>
+      </c>
+      <c r="M29" s="76">
+        <v>4.7139784946236558</v>
+      </c>
+      <c r="N29" s="76">
+        <v>4.715412186379929</v>
+      </c>
     </row>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44">
+    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="78">
         <v>29</v>
       </c>
       <c r="B30" s="37">
@@ -13191,9 +13747,25 @@
         <f>VLOOKUP(D30,'Overall Rating'!C:G,5,FALSE)</f>
         <v>180</v>
       </c>
+      <c r="I30" s="62"/>
+      <c r="J30" s="66">
+        <v>56</v>
+      </c>
+      <c r="K30" s="64">
+        <v>4.7392857142857139</v>
+      </c>
+      <c r="L30" s="64">
+        <v>4.75</v>
+      </c>
+      <c r="M30" s="64">
+        <v>4.7285714285714286</v>
+      </c>
+      <c r="N30" s="64">
+        <v>4.7392857142857139</v>
+      </c>
     </row>
-    <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="44">
+    <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="78">
         <v>30</v>
       </c>
       <c r="B31" s="37">
@@ -13220,10 +13792,21 @@
         <f>VLOOKUP(D31,'Overall Rating'!C:G,5,FALSE)</f>
         <v>208</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="43" t="s">
-        <v>85</v>
+      <c r="I31" s="62"/>
+      <c r="J31" s="66">
+        <v>113</v>
+      </c>
+      <c r="K31" s="64">
+        <v>4.7451327433628316</v>
+      </c>
+      <c r="L31" s="64">
+        <v>4.7522123893805315</v>
+      </c>
+      <c r="M31" s="64">
+        <v>4.7292035398230095</v>
+      </c>
+      <c r="N31" s="64">
+        <v>4.7421828908554575</v>
       </c>
     </row>
   </sheetData>
@@ -13232,7 +13815,7 @@
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13244,7 +13827,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13253,7 +13836,194 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L31">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{836F563A-26B8-484B-838F-82A0B2B48683}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Heatmap!K2:N2</xm:f>
+              <xm:sqref>O2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K3:N3</xm:f>
+              <xm:sqref>O3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K4:N4</xm:f>
+              <xm:sqref>O4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K5:N5</xm:f>
+              <xm:sqref>O5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K6:N6</xm:f>
+              <xm:sqref>O6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K7:N7</xm:f>
+              <xm:sqref>O7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K8:N8</xm:f>
+              <xm:sqref>O8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K9:N9</xm:f>
+              <xm:sqref>O9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K10:N10</xm:f>
+              <xm:sqref>O10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K11:N11</xm:f>
+              <xm:sqref>O11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K12:N12</xm:f>
+              <xm:sqref>O12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K13:N13</xm:f>
+              <xm:sqref>O13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K14:N14</xm:f>
+              <xm:sqref>O14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K15:N15</xm:f>
+              <xm:sqref>O15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K16:N16</xm:f>
+              <xm:sqref>O16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K17:N17</xm:f>
+              <xm:sqref>O17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K18:N18</xm:f>
+              <xm:sqref>O18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K19:N19</xm:f>
+              <xm:sqref>O19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K20:N20</xm:f>
+              <xm:sqref>O20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K21:N21</xm:f>
+              <xm:sqref>O21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K22:N22</xm:f>
+              <xm:sqref>O22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K23:N23</xm:f>
+              <xm:sqref>O23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K24:N24</xm:f>
+              <xm:sqref>O24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K25:N25</xm:f>
+              <xm:sqref>O25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K26:N26</xm:f>
+              <xm:sqref>O26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K27:N27</xm:f>
+              <xm:sqref>O27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K28:N28</xm:f>
+              <xm:sqref>O28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K29:N29</xm:f>
+              <xm:sqref>O29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K30:N30</xm:f>
+              <xm:sqref>O30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Heatmap!K31:N31</xm:f>
+              <xm:sqref>O31</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13261,620 +14031,620 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1221C93F-E779-40E4-A87E-E18B78CB8C2F}">
   <dimension ref="A3:G40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C30" sqref="C30:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.25" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="45"/>
+    <col min="1" max="1" width="50.25" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.25" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="44"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="45" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="46" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="48">
         <v>2</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="49">
         <v>0.59716389322148222</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="49">
         <v>0.95995278644296433</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="49">
         <v>0.234375</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="50">
         <v>7.9649059944355454</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="48">
         <v>1</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="49">
         <v>0.234375</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>0.234375</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="49">
         <v>0.234375</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="50">
         <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="48">
         <v>1</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="49">
         <v>0.95995278644296433</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="49">
         <v>0.95995278644296433</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="49">
         <v>0.95995278644296433</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="50">
         <v>9.4298119888710907</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="48">
         <v>3</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="49">
         <v>0.88299303759280801</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="49">
         <v>0.91862567811934903</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="49">
         <v>0.8598798970546182</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="50">
         <v>9.0765684274691676</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="48">
         <v>3</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="49">
         <v>0.95098039215686281</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="49">
         <v>1</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="49">
         <v>0.8529411764705882</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="50">
         <v>9.5425696594427247</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="48">
         <v>2</v>
       </c>
-      <c r="C9" s="50">
+      <c r="C9" s="49">
         <v>0.9291912530371399</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="49">
         <v>0.93798449612403101</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="49">
         <v>0.92039800995024879</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="50">
         <v>9.2990859655212326</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="48">
         <v>3</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="49">
         <v>0.94438288783702917</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="49">
         <v>0.99358974358974361</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="49">
         <v>0.91901408450704225</v>
       </c>
-      <c r="F10" s="51">
+      <c r="F10" s="50">
         <v>9.4702830182878461</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="48">
         <v>2</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="49">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="49">
         <v>0.76388888888888895</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="49">
         <v>0.5</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="50">
         <v>8.1101190476190474</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="48">
         <v>1</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="49">
         <v>0.94971537001897532</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="49">
         <v>0.94971537001897532</v>
       </c>
-      <c r="E12" s="50">
+      <c r="E12" s="49">
         <v>0.94971537001897532</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="50">
         <v>9.4449715370018978</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="48">
         <v>2</v>
       </c>
-      <c r="C13" s="50">
+      <c r="C13" s="49">
         <v>0.80036892805902848</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="49">
         <v>0.87804878048780488</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="49">
         <v>0.72268907563025209</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="50">
         <v>8.782588645214183</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="48">
         <v>1</v>
       </c>
-      <c r="C14" s="50">
+      <c r="C14" s="49">
         <v>0.87804878048780488</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="49">
         <v>0.87804878048780488</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="49">
         <v>0.87804878048780488</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="50">
         <v>9.0609756097560972</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="48">
         <v>1</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="49">
         <v>0.72268907563025209</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="49">
         <v>0.72268907563025209</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="49">
         <v>0.72268907563025209</v>
       </c>
-      <c r="F15" s="51">
+      <c r="F15" s="50">
         <v>8.5042016806722689</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="48">
         <v>2</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="49">
         <v>0.8854803493449781</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="49">
         <v>0.95</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="49">
         <v>0.82096069868995636</v>
       </c>
-      <c r="F16" s="51">
+      <c r="F16" s="50">
         <v>9.1519650655021838</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="48">
         <v>1</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="49">
         <v>0.95</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="49">
         <v>0.95</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="49">
         <v>0.95</v>
       </c>
-      <c r="F17" s="51">
+      <c r="F17" s="50">
         <v>9.4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="48">
         <v>1</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="49">
         <v>0.82096069868995636</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="49">
         <v>0.82096069868995636</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="49">
         <v>0.82096069868995636</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="50">
         <v>8.9039301310043673</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="48">
         <v>10</v>
       </c>
-      <c r="C19" s="50">
+      <c r="C19" s="49">
         <v>0.94163829493251883</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="49">
         <v>0.97115384615384615</v>
       </c>
-      <c r="E19" s="50">
+      <c r="E19" s="49">
         <v>0.88725490196078427</v>
       </c>
-      <c r="F19" s="51">
+      <c r="F19" s="50">
         <v>9.4158198258436308</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="52" t="s">
+      <c r="G30" s="61" t="s">
         <v>90</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="54">
+      <c r="B31" s="53">
         <v>2</v>
       </c>
-      <c r="C31" s="55">
+      <c r="C31" s="54">
         <v>0.59716389322148222</v>
       </c>
-      <c r="D31" s="55">
+      <c r="D31" s="54">
         <v>0.95995278644296433</v>
       </c>
-      <c r="E31" s="55">
+      <c r="E31" s="54">
         <v>0.234375</v>
       </c>
-      <c r="F31" s="56">
+      <c r="F31" s="55">
         <v>7.9649059944355454</v>
       </c>
-      <c r="G31" s="62">
+      <c r="G31" s="61">
         <f t="shared" ref="G31:G40" si="0">RANK(C31,$C$31:$C$40)</f>
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="54">
+      <c r="B32" s="53">
         <v>3</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="54">
         <v>0.88299303759280801</v>
       </c>
-      <c r="D32" s="55">
+      <c r="D32" s="54">
         <v>0.91862567811934903</v>
       </c>
-      <c r="E32" s="55">
+      <c r="E32" s="54">
         <v>0.8598798970546182</v>
       </c>
-      <c r="F32" s="56">
+      <c r="F32" s="55">
         <v>9.0765684274691676</v>
       </c>
-      <c r="G32" s="62">
+      <c r="G32" s="61">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="54">
+      <c r="B33" s="53">
         <v>3</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <v>0.95098039215686281</v>
       </c>
-      <c r="D33" s="55">
+      <c r="D33" s="54">
         <v>1</v>
       </c>
-      <c r="E33" s="55">
+      <c r="E33" s="54">
         <v>0.8529411764705882</v>
       </c>
-      <c r="F33" s="56">
+      <c r="F33" s="55">
         <v>9.5425696594427247</v>
       </c>
-      <c r="G33" s="62">
+      <c r="G33" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="54">
+      <c r="B34" s="53">
         <v>2</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>0.9291912530371399</v>
       </c>
-      <c r="D34" s="55">
+      <c r="D34" s="54">
         <v>0.93798449612403101</v>
       </c>
-      <c r="E34" s="55">
+      <c r="E34" s="54">
         <v>0.92039800995024879</v>
       </c>
-      <c r="F34" s="56">
+      <c r="F34" s="55">
         <v>9.2990859655212326</v>
       </c>
-      <c r="G34" s="62">
+      <c r="G34" s="61">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="54">
+      <c r="B35" s="53">
         <v>3</v>
       </c>
-      <c r="C35" s="55">
+      <c r="C35" s="54">
         <v>0.94438288783702917</v>
       </c>
-      <c r="D35" s="55">
+      <c r="D35" s="54">
         <v>0.99358974358974361</v>
       </c>
-      <c r="E35" s="55">
+      <c r="E35" s="54">
         <v>0.91901408450704225</v>
       </c>
-      <c r="F35" s="56">
+      <c r="F35" s="55">
         <v>9.4702830182878461</v>
       </c>
-      <c r="G35" s="62">
+      <c r="G35" s="61">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="54">
+      <c r="B36" s="53">
         <v>2</v>
       </c>
-      <c r="C36" s="55">
+      <c r="C36" s="54">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D36" s="55">
+      <c r="D36" s="54">
         <v>0.76388888888888895</v>
       </c>
-      <c r="E36" s="55">
+      <c r="E36" s="54">
         <v>0.5</v>
       </c>
-      <c r="F36" s="56">
+      <c r="F36" s="55">
         <v>8.1101190476190474</v>
       </c>
-      <c r="G36" s="62">
+      <c r="G36" s="61">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="54">
+      <c r="B37" s="53">
         <v>1</v>
       </c>
-      <c r="C37" s="55">
+      <c r="C37" s="54">
         <v>0.94971537001897532</v>
       </c>
-      <c r="D37" s="55">
+      <c r="D37" s="54">
         <v>0.94971537001897532</v>
       </c>
-      <c r="E37" s="55">
+      <c r="E37" s="54">
         <v>0.94971537001897532</v>
       </c>
-      <c r="F37" s="56">
+      <c r="F37" s="55">
         <v>9.4449715370018978</v>
       </c>
-      <c r="G37" s="62">
+      <c r="G37" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="54">
+      <c r="B38" s="53">
         <v>2</v>
       </c>
-      <c r="C38" s="55">
+      <c r="C38" s="54">
         <v>0.80036892805902848</v>
       </c>
-      <c r="D38" s="55">
+      <c r="D38" s="54">
         <v>0.87804878048780488</v>
       </c>
-      <c r="E38" s="55">
+      <c r="E38" s="54">
         <v>0.72268907563025209</v>
       </c>
-      <c r="F38" s="56">
+      <c r="F38" s="55">
         <v>8.782588645214183</v>
       </c>
-      <c r="G38" s="62">
+      <c r="G38" s="61">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="54">
+      <c r="B39" s="53">
         <v>2</v>
       </c>
-      <c r="C39" s="55">
+      <c r="C39" s="54">
         <v>0.8854803493449781</v>
       </c>
-      <c r="D39" s="55">
+      <c r="D39" s="54">
         <v>0.95</v>
       </c>
-      <c r="E39" s="55">
+      <c r="E39" s="54">
         <v>0.82096069868995636</v>
       </c>
-      <c r="F39" s="56">
+      <c r="F39" s="55">
         <v>9.1519650655021838</v>
       </c>
-      <c r="G39" s="62">
+      <c r="G39" s="61">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="58">
+      <c r="B40" s="57">
         <v>10</v>
       </c>
-      <c r="C40" s="59">
+      <c r="C40" s="58">
         <v>0.94163829493251883</v>
       </c>
-      <c r="D40" s="59">
+      <c r="D40" s="58">
         <v>0.97115384615384615</v>
       </c>
-      <c r="E40" s="59">
+      <c r="E40" s="58">
         <v>0.88725490196078427</v>
       </c>
-      <c r="F40" s="60">
+      <c r="F40" s="59">
         <v>9.4158198258436308</v>
       </c>
-      <c r="G40" s="62">
+      <c r="G40" s="61">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>

</xml_diff>